<commit_message>
add invoice_sheet_functions.py, test file, test_invoice_data.xlsx
</commit_message>
<xml_diff>
--- a/src/python/comp-230/invoice_data.xlsx
+++ b/src/python/comp-230/invoice_data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="-15" windowWidth="14400" windowHeight="12240" activeTab="2"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="14400" windowHeight="12240" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Customers" sheetId="1" r:id="rId1"/>
@@ -1566,7 +1566,7 @@
   <dimension ref="A1:K37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2321,7 +2321,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
@@ -3004,10 +3004,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R82"/>
+  <dimension ref="A1:R83"/>
   <sheetViews>
-    <sheetView topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="C89" sqref="C89"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3096,13 +3096,13 @@
     </row>
     <row r="4" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B4" s="7">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C4" s="9">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
@@ -3125,7 +3125,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="7">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C5" s="9">
         <v>1</v>
@@ -3148,13 +3148,13 @@
     </row>
     <row r="6" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="7">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B6" s="7">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C6" s="9">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
@@ -3177,10 +3177,10 @@
         <v>3</v>
       </c>
       <c r="B7" s="7">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="C7" s="9">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
@@ -3200,13 +3200,13 @@
     </row>
     <row r="8" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B8" s="7">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C8" s="9">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
@@ -3229,10 +3229,10 @@
         <v>4</v>
       </c>
       <c r="B9" s="7">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="C9" s="9">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
@@ -3252,13 +3252,13 @@
     </row>
     <row r="10" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="7">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B10" s="7">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C10" s="9">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
@@ -3281,10 +3281,10 @@
         <v>5</v>
       </c>
       <c r="B11" s="7">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="C11" s="9">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
@@ -3304,13 +3304,13 @@
     </row>
     <row r="12" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="7">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B12" s="7">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C12" s="9">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
@@ -3333,10 +3333,10 @@
         <v>6</v>
       </c>
       <c r="B13" s="7">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C13" s="9">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
@@ -3356,13 +3356,13 @@
     </row>
     <row r="14" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="7">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B14" s="7">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C14" s="9">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
@@ -3385,10 +3385,10 @@
         <v>7</v>
       </c>
       <c r="B15" s="7">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="C15" s="9">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
@@ -3408,13 +3408,13 @@
     </row>
     <row r="16" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="7">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B16" s="7">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C16" s="9">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
@@ -3437,10 +3437,10 @@
         <v>8</v>
       </c>
       <c r="B17" s="7">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C17" s="9">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
@@ -3460,13 +3460,13 @@
     </row>
     <row r="18" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="7">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B18" s="7">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="C18" s="9">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
@@ -3489,10 +3489,10 @@
         <v>9</v>
       </c>
       <c r="B19" s="7">
+        <v>13</v>
+      </c>
+      <c r="C19" s="9">
         <v>1</v>
-      </c>
-      <c r="C19" s="9">
-        <v>12</v>
       </c>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
@@ -3512,13 +3512,13 @@
     </row>
     <row r="20" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="7">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B20" s="7">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="C20" s="9">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
@@ -3541,10 +3541,10 @@
         <v>10</v>
       </c>
       <c r="B21" s="7">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C21" s="9">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
@@ -3564,13 +3564,13 @@
     </row>
     <row r="22" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="7">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B22" s="7">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C22" s="9">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
@@ -3593,10 +3593,10 @@
         <v>11</v>
       </c>
       <c r="B23" s="7">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C23" s="9">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
@@ -3616,13 +3616,13 @@
     </row>
     <row r="24" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="7">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B24" s="7">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C24" s="9">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
@@ -3645,10 +3645,10 @@
         <v>12</v>
       </c>
       <c r="B25" s="7">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="C25" s="9">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
@@ -3668,13 +3668,13 @@
     </row>
     <row r="26" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="7">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B26" s="7">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="C26" s="9">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
@@ -3697,10 +3697,10 @@
         <v>13</v>
       </c>
       <c r="B27" s="7">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C27" s="9">
-        <v>76</v>
+        <v>10</v>
       </c>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
@@ -3720,13 +3720,13 @@
     </row>
     <row r="28" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="7">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B28" s="7">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="C28" s="9">
-        <v>1</v>
+        <v>76</v>
       </c>
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
@@ -3749,10 +3749,10 @@
         <v>14</v>
       </c>
       <c r="B29" s="7">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C29" s="9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
@@ -3772,13 +3772,13 @@
     </row>
     <row r="30" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="7">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B30" s="7">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="C30" s="9">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
@@ -3801,10 +3801,10 @@
         <v>15</v>
       </c>
       <c r="B31" s="7">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C31" s="9">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
@@ -3824,13 +3824,13 @@
     </row>
     <row r="32" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" s="7">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B32" s="7">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="C32" s="9">
-        <v>42</v>
+        <v>10</v>
       </c>
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
@@ -3853,10 +3853,10 @@
         <v>16</v>
       </c>
       <c r="B33" s="7">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C33" s="9">
-        <v>19</v>
+        <v>42</v>
       </c>
       <c r="D33" s="1"/>
       <c r="E33" s="1"/>
@@ -3876,13 +3876,13 @@
     </row>
     <row r="34" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34" s="7">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B34" s="7">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C34" s="9">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
@@ -3905,10 +3905,10 @@
         <v>17</v>
       </c>
       <c r="B35" s="7">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="C35" s="9">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="D35" s="1"/>
       <c r="E35" s="1"/>
@@ -3928,13 +3928,13 @@
     </row>
     <row r="36" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" s="7">
-        <v>17.710526315789501</v>
+        <v>17</v>
       </c>
       <c r="B36" s="7">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="C36" s="9">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="D36" s="1"/>
       <c r="E36" s="1"/>
@@ -3954,65 +3954,80 @@
     </row>
     <row r="37" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A37" s="7">
-        <v>18.206766917293201</v>
-      </c>
-      <c r="B37" s="15">
-        <v>8</v>
-      </c>
-      <c r="C37" s="16">
-        <v>1</v>
-      </c>
+        <v>17.710526315789501</v>
+      </c>
+      <c r="B37" s="7">
+        <v>9</v>
+      </c>
+      <c r="C37" s="9">
+        <v>15</v>
+      </c>
+      <c r="D37" s="1"/>
+      <c r="E37" s="1"/>
+      <c r="F37" s="1"/>
+      <c r="G37" s="1"/>
+      <c r="H37" s="1"/>
+      <c r="I37" s="1"/>
+      <c r="J37" s="1"/>
+      <c r="K37" s="1"/>
+      <c r="L37" s="1"/>
+      <c r="M37" s="1"/>
+      <c r="N37" s="1"/>
+      <c r="O37" s="1"/>
+      <c r="P37" s="1"/>
+      <c r="Q37" s="1"/>
+      <c r="R37" s="1"/>
     </row>
     <row r="38" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" s="7">
-        <v>18.703007518797001</v>
+        <v>18.206766917293201</v>
       </c>
       <c r="B38" s="15">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C38" s="16">
-        <v>24</v>
+        <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A39" s="7">
-        <v>19.199248120300801</v>
+        <v>18.703007518797001</v>
       </c>
       <c r="B39" s="15">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C39" s="16">
-        <v>4</v>
+        <v>24</v>
       </c>
     </row>
     <row r="40" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A40" s="7">
-        <v>19.695488721804502</v>
+        <v>19.199248120300801</v>
       </c>
       <c r="B40" s="15">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="C40" s="16">
-        <v>15</v>
+        <v>4</v>
       </c>
     </row>
     <row r="41" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A41" s="7">
-        <v>20.191729323308302</v>
+        <v>19.695488721804502</v>
       </c>
       <c r="B41" s="15">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="C41" s="16">
-        <v>3</v>
+        <v>15</v>
       </c>
     </row>
     <row r="42" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A42" s="7">
-        <v>20.687969924811998</v>
+        <v>20.191729323308302</v>
       </c>
       <c r="B42" s="15">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C42" s="16">
         <v>3</v>
@@ -4020,347 +4035,355 @@
     </row>
     <row r="43" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A43" s="7">
-        <v>21.184210526315798</v>
+        <v>20.687969924811998</v>
       </c>
       <c r="B43" s="15">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="C43" s="16">
-        <v>19</v>
+        <v>3</v>
       </c>
     </row>
     <row r="44" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A44" s="7">
-        <v>21.680451127819602</v>
+        <v>21.184210526315798</v>
       </c>
       <c r="B44" s="15">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C44" s="16">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="45" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A45" s="7">
-        <v>22.176691729323299</v>
+        <v>21.680451127819602</v>
       </c>
       <c r="B45" s="15">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="C45" s="16">
-        <v>7</v>
+        <v>23</v>
       </c>
     </row>
     <row r="46" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A46" s="7">
-        <v>22.672932330827098</v>
+        <v>22.176691729323299</v>
       </c>
       <c r="B46" s="15">
+        <v>11</v>
+      </c>
+      <c r="C46" s="16">
         <v>7</v>
-      </c>
-      <c r="C46" s="16">
-        <v>14</v>
       </c>
     </row>
     <row r="47" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A47" s="7">
-        <v>23.169172932330799</v>
+        <v>22.672932330827098</v>
       </c>
       <c r="B47" s="15">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C47" s="16">
-        <v>3</v>
+        <v>14</v>
       </c>
     </row>
     <row r="48" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A48" s="7">
-        <v>23.665413533834599</v>
+        <v>23.169172932330799</v>
       </c>
       <c r="B48" s="15">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="C48" s="16">
-        <v>14</v>
+        <v>3</v>
       </c>
     </row>
     <row r="49" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A49" s="7">
-        <v>24.161654135338399</v>
+        <v>23.665413533834599</v>
       </c>
       <c r="B49" s="15">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C49" s="16">
-        <v>9</v>
+        <v>14</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A50" s="7">
-        <v>24.657894736842099</v>
+        <v>24.161654135338399</v>
       </c>
       <c r="B50" s="15">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="C50" s="16">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="51" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A51" s="7">
-        <v>25.154135338345899</v>
+        <v>24.657894736842099</v>
       </c>
       <c r="B51" s="15">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C51" s="16">
-        <v>3</v>
+        <v>12</v>
       </c>
     </row>
     <row r="52" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A52" s="7">
-        <v>25.650375939849599</v>
+        <v>25.154135338345899</v>
       </c>
       <c r="B52" s="15">
+        <v>2</v>
+      </c>
+      <c r="C52" s="16">
         <v>3</v>
-      </c>
-      <c r="C52" s="16">
-        <v>48</v>
       </c>
     </row>
     <row r="53" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A53" s="7">
-        <v>26.146616541353399</v>
+        <v>25.650375939849599</v>
       </c>
       <c r="B53" s="15">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="C53" s="16">
-        <v>7</v>
+        <v>48</v>
       </c>
     </row>
     <row r="54" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A54" s="7">
-        <v>26.642857142857199</v>
+        <v>26.146616541353399</v>
       </c>
       <c r="B54" s="15">
+        <v>13</v>
+      </c>
+      <c r="C54" s="16">
         <v>7</v>
-      </c>
-      <c r="C54" s="16">
-        <v>34</v>
       </c>
     </row>
     <row r="55" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A55" s="7">
-        <v>27.1390977443609</v>
+        <v>26.642857142857199</v>
       </c>
       <c r="B55" s="15">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C55" s="16">
-        <v>4</v>
+        <v>34</v>
       </c>
     </row>
     <row r="56" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A56" s="7">
-        <v>27.6353383458647</v>
+        <v>27.1390977443609</v>
       </c>
       <c r="B56" s="15">
         <v>12</v>
       </c>
       <c r="C56" s="16">
-        <v>15</v>
+        <v>4</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A57" s="7">
-        <v>28.1315789473684</v>
+        <v>27.6353383458647</v>
       </c>
       <c r="B57" s="15">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="C57" s="16">
-        <v>4</v>
+        <v>15</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A58" s="7">
-        <v>28.6278195488722</v>
+        <v>28.1315789473684</v>
       </c>
       <c r="B58" s="15">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C58" s="16">
-        <v>21</v>
+        <v>4</v>
       </c>
     </row>
     <row r="59" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A59" s="7">
-        <v>29.124060150376</v>
+        <v>28.6278195488722</v>
       </c>
       <c r="B59" s="15">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C59" s="16">
-        <v>4</v>
+        <v>21</v>
       </c>
     </row>
     <row r="60" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A60" s="7">
-        <v>29.6203007518797</v>
+        <v>29.124060150376</v>
       </c>
       <c r="B60" s="15">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C60" s="16">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="61" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A61" s="7">
-        <v>30.1165413533835</v>
+        <v>29.6203007518797</v>
       </c>
       <c r="B61" s="15">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="C61" s="16">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="62" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A62" s="7">
-        <v>30.6127819548872</v>
+        <v>30.1165413533835</v>
       </c>
       <c r="B62" s="15">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C62" s="16">
-        <v>23</v>
+        <v>3</v>
       </c>
     </row>
     <row r="63" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A63" s="7">
-        <v>31.109022556391</v>
+        <v>30.6127819548872</v>
       </c>
       <c r="B63" s="15">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C63" s="16">
-        <v>4</v>
+        <v>23</v>
       </c>
     </row>
     <row r="64" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A64" s="7">
-        <v>31.6052631578948</v>
+        <v>31.109022556391</v>
       </c>
       <c r="B64" s="15">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C64" s="16">
-        <v>19</v>
+        <v>4</v>
       </c>
     </row>
     <row r="65" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A65" s="7">
-        <v>32.101503759398497</v>
+        <v>31.6052631578948</v>
       </c>
       <c r="B65" s="15">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C65" s="16">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="66" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A66" s="7">
-        <v>32.597744360902297</v>
+        <v>32.101503759398497</v>
       </c>
       <c r="B66" s="15">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C66" s="16">
-        <v>12</v>
+        <v>22</v>
       </c>
     </row>
     <row r="67" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A67" s="7">
-        <v>33.093984962405997</v>
+        <v>32.597744360902297</v>
       </c>
       <c r="B67" s="15">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C67" s="16">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="68" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A68" s="7">
-        <v>33.590225563909797</v>
+        <v>33.093984962405997</v>
       </c>
       <c r="B68" s="15">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C68" s="16">
-        <v>23</v>
+        <v>7</v>
       </c>
     </row>
     <row r="69" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A69" s="7">
-        <v>34.086466165413498</v>
+        <v>33.590225563909797</v>
       </c>
       <c r="B69" s="15">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="C69" s="16">
-        <v>1</v>
+        <v>23</v>
       </c>
     </row>
     <row r="70" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A70" s="7">
-        <v>34.582706766917298</v>
+        <v>34.086466165413498</v>
       </c>
       <c r="B70" s="15">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C70" s="16">
-        <v>42</v>
+        <v>1</v>
       </c>
     </row>
     <row r="71" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A71" s="7">
-        <v>35.078947368421098</v>
+        <v>34.582706766917298</v>
       </c>
       <c r="B71" s="15">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C71" s="16">
-        <v>7</v>
+        <v>42</v>
       </c>
     </row>
     <row r="72" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A72" s="7">
-        <v>35.575187969924798</v>
+        <v>35.078947368421098</v>
       </c>
       <c r="B72" s="15">
+        <v>6</v>
+      </c>
+      <c r="C72" s="16">
         <v>7</v>
-      </c>
-      <c r="C72" s="16">
-        <v>8</v>
       </c>
     </row>
     <row r="73" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A73" s="7">
+        <v>35.575187969924798</v>
+      </c>
+      <c r="B73" s="15">
+        <v>7</v>
+      </c>
+      <c r="C73" s="16">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A74" s="7">
         <v>36.071428571428598</v>
       </c>
-      <c r="B73" s="15">
+      <c r="B74" s="15">
         <v>1</v>
       </c>
-      <c r="C73" s="16">
+      <c r="C74" s="16">
         <v>1</v>
       </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A74" s="13"/>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" s="13"/>
@@ -4385,6 +4408,9 @@
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A82" s="13"/>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A83" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add invoice_printer func, sample inv, upd sheet_functions.py and test file
</commit_message>
<xml_diff>
--- a/src/python/comp-230/invoice_data.xlsx
+++ b/src/python/comp-230/invoice_data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="-15" windowWidth="14400" windowHeight="12240" activeTab="3"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="14400" windowHeight="12240" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Customers" sheetId="1" r:id="rId1"/>
@@ -1430,8 +1430,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K37"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C41" sqref="C41"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2186,7 +2186,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
@@ -2628,12 +2628,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="A74" sqref="A74:XFD74"/>
+    <sheetView topLeftCell="B40" workbookViewId="0">
+      <selection activeCell="B57" sqref="B57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="0" hidden="1" customWidth="1"/>
     <col min="2" max="4" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3346,13 +3347,13 @@
         <v>132</v>
       </c>
       <c r="B33" s="5">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="C33" s="5">
         <v>108</v>
       </c>
       <c r="D33" s="5">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>
@@ -3440,7 +3441,7 @@
         <v>109</v>
       </c>
       <c r="D37" s="5">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="E37" s="1"/>
       <c r="F37" s="1"/>
@@ -3722,13 +3723,13 @@
         <v>156</v>
       </c>
       <c r="B57" s="5">
-        <v>128</v>
+        <v>118</v>
       </c>
       <c r="C57" s="5">
         <v>113</v>
       </c>
       <c r="D57" s="5">
-        <v>15</v>
+        <v>6</v>
       </c>
     </row>
     <row r="58" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
upd invoice_generator.py - add file validation
</commit_message>
<xml_diff>
--- a/src/python/comp-230/invoice_data.xlsx
+++ b/src/python/comp-230/invoice_data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="-15" windowWidth="14400" windowHeight="12240" activeTab="2"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="14400" windowHeight="12240" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Customers" sheetId="1" r:id="rId1"/>
@@ -803,7 +803,7 @@
   <dimension ref="A1:L22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -812,7 +812,7 @@
     <col min="2" max="5" width="20.7109375" customWidth="1"/>
     <col min="6" max="6" width="30.7109375" customWidth="1"/>
     <col min="7" max="11" width="20.7109375" customWidth="1"/>
-    <col min="12" max="12" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="23.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
@@ -1428,10 +1428,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K37"/>
+  <dimension ref="A1:K48"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2177,6 +2177,39 @@
       </c>
       <c r="E37" s="3"/>
     </row>
+    <row r="38" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B38" s="5"/>
+    </row>
+    <row r="39" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B39" s="5"/>
+    </row>
+    <row r="40" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B40" s="5"/>
+    </row>
+    <row r="41" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B41" s="5"/>
+    </row>
+    <row r="42" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B42" s="5"/>
+    </row>
+    <row r="43" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B43" s="5"/>
+    </row>
+    <row r="44" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B44" s="5"/>
+    </row>
+    <row r="45" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B45" s="5"/>
+    </row>
+    <row r="46" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B46" s="5"/>
+    </row>
+    <row r="47" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B47" s="5"/>
+    </row>
+    <row r="48" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B48" s="5"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2186,8 +2219,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2628,13 +2661,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L73"/>
   <sheetViews>
-    <sheetView topLeftCell="B40" workbookViewId="0">
-      <selection activeCell="B57" sqref="B57"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="0" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" hidden="1" customWidth="1"/>
     <col min="2" max="4" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>